<commit_message>
chore: update intents files
</commit_message>
<xml_diff>
--- a/intents.xlsx
+++ b/intents.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">article</t>
   </si>
@@ -31,7 +31,10 @@
     <t xml:space="preserve">I want to buy a shirt</t>
   </si>
   <si>
-    <t xml:space="preserve">i want to buy some polos</t>
+    <t xml:space="preserve">i want to buy a products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I want to buy some jeans</t>
   </si>
   <si>
     <t xml:space="preserve">greetings</t>
@@ -148,10 +151,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -182,8 +185,8 @@
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>4</v>
       </c>
     </row>
@@ -195,6 +198,11 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>